<commit_message>
Update SUZ nCorner Sheet
</commit_message>
<xml_diff>
--- a/+Plotting/+nCorner/SUZ.xlsx
+++ b/+Plotting/+nCorner/SUZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Saian\Workspace\Data\+Plotting\+nCorner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2329967-3977-474A-B72D-C6C4B5A9D95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9AF1DF-92D7-44B0-86FD-D79A9DC20B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF94FF5B-EA6C-476F-8E8D-3CB1080C88ED}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="7800" xr2:uid="{FF94FF5B-EA6C-476F-8E8D-3CB1080C88ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +511,10 @@
         <v>630</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -540,10 +540,10 @@
         <v>645</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>875</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -569,10 +569,10 @@
         <v>400</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>875</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1040</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -598,10 +598,10 @@
         <v>340</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1040</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1190</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -627,10 +627,10 @@
         <v>170</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1190</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1380</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -656,10 +656,10 @@
         <v>40</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1380</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1580</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -685,10 +685,10 @@
         <v>-160</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1580</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1735</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -714,10 +714,10 @@
         <v>-260</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1735</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2020</v>
       </c>
       <c r="H9">
         <v>2</v>

</xml_diff>